<commit_message>
create mck api 3
</commit_message>
<xml_diff>
--- a/music_info.xlsx
+++ b/music_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eunjin/github/WeatherApp_iOS/Server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305052F1-32C5-F544-B527-62361D573F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E3DAD5-4617-7441-86E5-1C6FFEAB2235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1920" windowWidth="28800" windowHeight="16080" xr2:uid="{7E9501A6-B97A-B84E-95A0-978DF33FBD0A}"/>
+    <workbookView xWindow="32460" yWindow="2620" windowWidth="28800" windowHeight="16080" xr2:uid="{7E9501A6-B97A-B84E-95A0-978DF33FBD0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -919,7 +919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D340A-F097-2049-94E1-069D363D812B}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -979,9 +981,6 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1017,9 +1016,6 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1053,7 +1049,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>20</v>
@@ -1087,9 +1083,6 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1227,9 +1220,6 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
       <c r="C9" s="11" t="s">
         <v>63</v>
       </c>
@@ -1332,6 +1322,9 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>86</v>
       </c>
@@ -1364,6 +1357,9 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>93</v>
       </c>
@@ -1399,6 +1395,9 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>102</v>
       </c>
@@ -1433,6 +1432,9 @@
     <row r="15" spans="1:12" ht="19">
       <c r="A15" s="1">
         <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>109</v>

</xml_diff>